<commit_message>
remplissage de la documentation
</commit_message>
<xml_diff>
--- a/DOC/journaux.xlsx
+++ b/DOC/journaux.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\année 2017-2018\Modules I-CT\431\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Almir.RAZIC\Documents\GitHub\Bataille-navale\DOC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
   <si>
     <t>Journal de bord</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>aide aux autres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 min </t>
+  </si>
+  <si>
+    <t>création d'un repository,instalation de gihubdesktop et prise en main</t>
   </si>
 </sst>
 </file>
@@ -565,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -635,6 +641,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,7 +928,7 @@
   <dimension ref="B1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,11 +1283,21 @@
       <c r="F13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="3"/>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="15">
+        <v>43558</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="34" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="2:12" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">

</xml_diff>